<commit_message>
State functions, minimize columns in transition table
</commit_message>
<xml_diff>
--- a/PLATYPUS_Transition_Table.xlsx
+++ b/PLATYPUS_Transition_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="27">
   <si>
     <t>Current</t>
   </si>
@@ -53,6 +53,9 @@
     <t>other</t>
   </si>
   <si>
+    <t>[1-7]</t>
+  </si>
+  <si>
     <t>IS/ES</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
   </si>
   <si>
     <t>OIL - ASWR</t>
+  </si>
+  <si>
+    <t>[8-9]</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -175,11 +181,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -210,6 +253,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,26 +580,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="Z15" sqref="S15:Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="12" width="4.85546875" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" customWidth="1"/>
     <col min="16" max="16" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.5703125" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -562,7 +621,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -585,8 +644,24 @@
       <c r="P2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="R2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="14"/>
     </row>
-    <row r="3" spans="1:16" s="10" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="10" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -635,8 +710,36 @@
       <c r="P3" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="R3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="7">
+        <v>0</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="9"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -674,19 +777,47 @@
         <v>4</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="P4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5">
+        <v>6</v>
+      </c>
+      <c r="U4" s="5">
+        <v>4</v>
+      </c>
+      <c r="V4" s="1">
+        <v>4</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="Y4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -724,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N5" s="5">
         <v>3</v>
@@ -733,115 +864,199 @@
         <v>2</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="57" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="R6" s="3">
+        <v>2</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="R7" s="3">
+        <v>3</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5">
         <v>4</v>
@@ -883,65 +1098,121 @@
         <v>5</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R8" s="3">
+        <v>4</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8" s="5">
+        <v>4</v>
+      </c>
+      <c r="U8" s="5">
+        <v>4</v>
+      </c>
+      <c r="V8" s="1">
+        <v>4</v>
+      </c>
+      <c r="W8" s="5">
+        <v>7</v>
+      </c>
+      <c r="X8" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="5"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="R9" s="3">
+        <v>5</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9" s="5"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5">
         <v>9</v>
@@ -968,30 +1239,58 @@
         <v>9</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M10" s="5">
         <v>7</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O10" s="5">
         <v>5</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R10" s="3">
+        <v>6</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" s="5">
+        <v>9</v>
+      </c>
+      <c r="U10" s="5">
+        <v>9</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" s="5">
+        <v>7</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5">
         <v>7</v>
@@ -1024,7 +1323,7 @@
         <v>7</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N11" s="5">
         <v>8</v>
@@ -1033,65 +1332,121 @@
         <v>8</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R11" s="3">
+        <v>7</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="5">
+        <v>7</v>
+      </c>
+      <c r="U11" s="5">
+        <v>7</v>
+      </c>
+      <c r="V11" s="1">
+        <v>7</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X11" s="5">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA11" s="5"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="R12" s="3">
+        <v>8</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA12" s="5"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5">
         <v>9</v>
@@ -1118,228 +1473,359 @@
         <v>9</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O13" s="5">
         <v>10</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="R13" s="3">
+        <v>9</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T13" s="5">
+        <v>9</v>
+      </c>
+      <c r="U13" s="5">
+        <v>9</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>10</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="R14" s="3">
+        <v>10</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA14" s="5"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="R15" s="3">
+        <v>11</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="5"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="R16" s="3">
+        <v>12</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA16" s="5"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="3">
         <v>13</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="S17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA17" s="5"/>
+    </row>
+    <row r="19" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="A1:P1"/>
+    <mergeCell ref="S2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix transition table. Need to fix string literal read
</commit_message>
<xml_diff>
--- a/PLATYPUS_Transition_Table.xlsx
+++ b/PLATYPUS_Transition_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="27">
   <si>
     <t>Current</t>
   </si>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z15" sqref="S15:Z15"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
       </c>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="AA6" s="5"/>
     </row>
-    <row r="7" spans="1:27" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="AA8" s="5"/>
     </row>
-    <row r="9" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1349,8 +1349,8 @@
       <c r="V11" s="1">
         <v>7</v>
       </c>
-      <c r="W11" s="5" t="s">
-        <v>20</v>
+      <c r="W11" s="5">
+        <v>8</v>
       </c>
       <c r="X11" s="5">
         <v>8</v>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="AA11" s="5"/>
     </row>
-    <row r="12" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="AA13" s="5"/>
     </row>
-    <row r="14" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="5"/>
     </row>
-    <row r="16" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="AA16" s="5"/>
     </row>
-    <row r="17" spans="1:27" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>13</v>
       </c>

</xml_diff>